<commit_message>
add details sheet to the Annual Report excel file
</commit_message>
<xml_diff>
--- a/AnnualReports.Web/Content/ExcelTemplates/AnnualReportTemplate.xlsx
+++ b/AnnualReports.Web/Content/ExcelTemplates/AnnualReportTemplate.xlsx
@@ -13,13 +13,14 @@
   </bookViews>
   <sheets>
     <sheet name="Schedule 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Details" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Year</t>
   </si>
@@ -40,6 +41,33 @@
   </si>
   <si>
     <t>Amount</t>
+  </si>
+  <si>
+    <t>Debit</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>Account Description</t>
+  </si>
+  <si>
+    <t>Act #1</t>
+  </si>
+  <si>
+    <t>Act #2</t>
+  </si>
+  <si>
+    <t>Act #3</t>
+  </si>
+  <si>
+    <t>Act #4</t>
+  </si>
+  <si>
+    <t>Act #5</t>
   </si>
 </sst>
 </file>
@@ -431,7 +459,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -441,8 +472,8 @@
     <col min="4" max="4" width="32.88671875" style="2" customWidth="1"/>
     <col min="5" max="5" width="17.21875" customWidth="1"/>
     <col min="6" max="6" width="32" customWidth="1"/>
-    <col min="7" max="7" width="17.88671875" style="4" customWidth="1"/>
-    <col min="8" max="21" width="7.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.77734375" style="4" customWidth="1"/>
+    <col min="8" max="20" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -473,4 +504,69 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
hide "Period" column from UI.
</commit_message>
<xml_diff>
--- a/AnnualReports.Web/Content/ExcelTemplates/AnnualReportTemplate.xlsx
+++ b/AnnualReports.Web/Content/ExcelTemplates/AnnualReportTemplate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Year</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Credit</t>
-  </si>
-  <si>
-    <t>Period</t>
   </si>
   <si>
     <t>Account Description</t>
@@ -508,7 +505,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -524,48 +521,44 @@
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="14.109375" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" customWidth="1"/>
-    <col min="9" max="9" width="16.88671875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>9</v>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Display BARS Code in annual report.
</commit_message>
<xml_diff>
--- a/AnnualReports.Web/Content/ExcelTemplates/AnnualReportTemplate.xlsx
+++ b/AnnualReports.Web/Content/ExcelTemplates/AnnualReportTemplate.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Year</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Act #5</t>
+  </si>
+  <si>
+    <t>BARS Code</t>
   </si>
 </sst>
 </file>
@@ -456,9 +459,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -505,9 +508,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -515,18 +518,18 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" style="4" customWidth="1"/>
+    <col min="2" max="3" width="32.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -534,31 +537,34 @@
         <v>9</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>